<commit_message>
Cambios finales para la maquina1 en el word
</commit_message>
<xml_diff>
--- a/Docs/Tablas Lab 4.xlsx
+++ b/Docs/Tablas Lab 4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\OneDrive\Documentos\Universidad\Segundo Semestre\EDA\Retos\Reto1\Reto1-G01T\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{674F579C-51C2-4508-8FD2-09D1C34F07F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E680D4DC-9C4F-4AC8-87C8-5E355D09751D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Lab4" sheetId="1" r:id="rId1"/>
@@ -130,7 +130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -144,6 +144,7 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -661,37 +662,25 @@
             <c:numRef>
               <c:f>'Datos Lab4'!$B$2:$B$11</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>796.88</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>3234.38</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>12828.13</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>51750.05</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50</c:v>
+                  <c:v>214515.22</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>100</c:v>
+                  <c:v>943625.99</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -829,37 +818,25 @@
             <c:numRef>
               <c:f>'Datos Lab4'!$C$2:$C$11</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>578.13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2265.63</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>9125.69</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>38125.06</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>1688593.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>89</c:v>
+                  <c:v>724437.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -996,37 +973,34 @@
             <c:numRef>
               <c:f>'Datos Lab4'!$D$2:$D$11</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>31.79</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19</c:v>
+                  <c:v>62.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29</c:v>
+                  <c:v>156.33000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39</c:v>
+                  <c:v>343.44</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49</c:v>
+                  <c:v>812.53</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>59</c:v>
+                  <c:v>1796.21</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>69</c:v>
+                  <c:v>4390.53</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>79</c:v>
+                  <c:v>10750.22</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>89</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>99</c:v>
+                  <c:v>26250.16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1252,7 +1226,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1576,37 +1550,13 @@
             <c:numRef>
               <c:f>'Datos Lab4'!$B$15:$B$24</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>50</c:v>
+                  <c:v>30734.38</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>140</c:v>
+                  <c:v>258234.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1705,37 +1655,13 @@
             <c:numRef>
               <c:f>'Datos Lab4'!$C$15:$C$24</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>30640.91</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>178</c:v>
+                  <c:v>280906.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1744,37 +1670,13 @@
             <c:numRef>
               <c:f>'Datos Lab4'!$C$15:$C$24</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>30640.91</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>178</c:v>
+                  <c:v>280906.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1911,37 +1813,19 @@
             <c:numRef>
               <c:f>'Datos Lab4'!$D$15:$D$24</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>1848.96</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78</c:v>
+                  <c:v>7781.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>88</c:v>
+                  <c:v>37382.81</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>108</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>118</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>138</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>148</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>158</c:v>
+                  <c:v>232937.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2167,7 +2051,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2492,37 +2376,25 @@
             <c:numRef>
               <c:f>'Datos Lab4'!$B$2:$B$11</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>796.88</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>3234.38</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>12828.13</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>51750.05</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50</c:v>
+                  <c:v>214515.22</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>100</c:v>
+                  <c:v>943625.99</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2660,37 +2532,13 @@
             <c:numRef>
               <c:f>'Datos Lab4'!$B$15:$B$24</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>50</c:v>
+                  <c:v>30734.38</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>140</c:v>
+                  <c:v>258234.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2911,7 +2759,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3231,37 +3079,25 @@
             <c:numRef>
               <c:f>'Datos Lab4'!$C$2:$C$11</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>578.13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2265.63</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>9125.69</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>38125.06</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>1688593.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>89</c:v>
+                  <c:v>724437.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3399,37 +3235,13 @@
             <c:numRef>
               <c:f>'Datos Lab4'!$C$15:$C$24</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>30640.91</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>178</c:v>
+                  <c:v>280906.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3650,7 +3462,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3970,37 +3782,34 @@
             <c:numRef>
               <c:f>'Datos Lab4'!$D$2:$D$11</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>31.79</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19</c:v>
+                  <c:v>62.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29</c:v>
+                  <c:v>156.33000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39</c:v>
+                  <c:v>343.44</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49</c:v>
+                  <c:v>812.53</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>59</c:v>
+                  <c:v>1796.21</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>69</c:v>
+                  <c:v>4390.53</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>79</c:v>
+                  <c:v>10750.22</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>89</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>99</c:v>
+                  <c:v>26250.16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4138,37 +3947,19 @@
             <c:numRef>
               <c:f>'Datos Lab4'!$D$15:$D$24</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>1848.96</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78</c:v>
+                  <c:v>7781.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>88</c:v>
+                  <c:v>37382.81</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>108</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>118</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>138</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>148</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>158</c:v>
+                  <c:v>232937.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4389,7 +4180,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -7286,7 +7077,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{BF2A59F4-6CD8-490D-818C-7B3BB3F2B140}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="86" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7297,7 +7088,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{0D09CF8B-80E2-4734-A9D4-9F6060F1BA3D}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="86" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7828,7 +7619,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4"/>
@@ -7857,158 +7648,123 @@
       <c r="A2" s="1">
         <v>1000</v>
       </c>
-      <c r="B2" s="4">
-        <v>10</v>
+      <c r="B2" s="5">
+        <v>796.88</v>
       </c>
-      <c r="C2" s="4">
-        <v>1</v>
+      <c r="C2" s="5">
+        <v>578.13</v>
       </c>
-      <c r="D2" s="4">
-        <v>4</v>
+      <c r="D2" s="5">
+        <v>31.79</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>2000</v>
       </c>
-      <c r="B3" s="4">
-        <v>20</v>
+      <c r="B3" s="5">
+        <v>3234.38</v>
       </c>
-      <c r="C3" s="4">
-        <v>2</v>
+      <c r="C3" s="5">
+        <v>2265.63</v>
       </c>
-      <c r="D3" s="4">
-        <f>D2+15</f>
-        <v>19</v>
+      <c r="D3" s="5">
+        <v>62.5</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>4000</v>
       </c>
-      <c r="B4" s="4">
-        <v>30</v>
+      <c r="B4" s="5">
+        <v>12828.13</v>
       </c>
-      <c r="C4" s="4">
-        <f>C3+C2</f>
-        <v>3</v>
+      <c r="C4" s="5">
+        <v>9125.69</v>
       </c>
-      <c r="D4" s="4">
-        <f t="shared" ref="D4:D11" si="0">D3+10</f>
-        <v>29</v>
+      <c r="D4" s="5">
+        <v>156.33000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>8000</v>
       </c>
-      <c r="B5" s="4">
-        <v>40</v>
+      <c r="B5" s="5">
+        <v>51750.05</v>
       </c>
-      <c r="C5" s="4">
-        <f t="shared" ref="C5:C11" si="1">C4+C3</f>
-        <v>5</v>
+      <c r="C5" s="5">
+        <v>38125.06</v>
       </c>
-      <c r="D5" s="4">
-        <f t="shared" si="0"/>
-        <v>39</v>
+      <c r="D5" s="5">
+        <v>343.44</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>16000</v>
       </c>
-      <c r="B6" s="4">
-        <v>50</v>
+      <c r="B6" s="5">
+        <v>214515.22</v>
       </c>
-      <c r="C6" s="4">
-        <f t="shared" si="1"/>
-        <v>8</v>
+      <c r="C6" s="5">
+        <v>1688593.75</v>
       </c>
-      <c r="D6" s="4">
-        <f t="shared" si="0"/>
-        <v>49</v>
+      <c r="D6" s="5">
+        <v>812.53</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>32000</v>
       </c>
-      <c r="B7" s="4">
-        <v>60</v>
+      <c r="B7" s="5">
+        <v>943625.99</v>
       </c>
-      <c r="C7" s="4">
-        <f t="shared" si="1"/>
-        <v>13</v>
+      <c r="C7" s="5">
+        <v>724437.5</v>
       </c>
-      <c r="D7" s="4">
-        <f t="shared" si="0"/>
-        <v>59</v>
+      <c r="D7" s="5">
+        <v>1796.21</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>64000</v>
       </c>
-      <c r="B8" s="4">
-        <v>70</v>
-      </c>
-      <c r="C8" s="4">
-        <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="D8" s="4">
-        <f t="shared" si="0"/>
-        <v>69</v>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="5">
+        <v>4390.53</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>128000</v>
       </c>
-      <c r="B9" s="4">
-        <v>80</v>
-      </c>
-      <c r="C9" s="4">
-        <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
-      <c r="D9" s="4">
-        <f t="shared" si="0"/>
-        <v>79</v>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="5">
+        <v>10750.22</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>256000</v>
       </c>
-      <c r="B10" s="4">
-        <v>90</v>
-      </c>
-      <c r="C10" s="4">
-        <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
-      <c r="D10" s="4">
-        <f t="shared" si="0"/>
-        <v>89</v>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="5">
+        <v>26250.16</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1">
         <v>512000</v>
       </c>
-      <c r="B11" s="4">
-        <v>100</v>
-      </c>
-      <c r="C11" s="4">
-        <f t="shared" si="1"/>
-        <v>89</v>
-      </c>
-      <c r="D11" s="4">
-        <f t="shared" si="0"/>
-        <v>99</v>
-      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
@@ -8028,158 +7784,97 @@
       <c r="A15" s="1">
         <v>1000</v>
       </c>
-      <c r="B15" s="4">
-        <v>50</v>
+      <c r="B15" s="5">
+        <v>30734.38</v>
       </c>
-      <c r="C15" s="4">
-        <v>2</v>
+      <c r="C15" s="5">
+        <v>30640.91</v>
       </c>
-      <c r="D15" s="4">
-        <v>35</v>
+      <c r="D15" s="5">
+        <v>1848.96</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1">
         <v>2000</v>
       </c>
-      <c r="B16" s="4">
-        <v>60</v>
+      <c r="B16" s="5">
+        <v>258234.3</v>
       </c>
-      <c r="C16" s="4">
-        <v>4</v>
+      <c r="C16" s="5">
+        <v>280906.3</v>
       </c>
-      <c r="D16" s="4">
-        <f>D15+43</f>
-        <v>78</v>
+      <c r="D16" s="5">
+        <v>7781.25</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1">
         <v>4000</v>
       </c>
-      <c r="B17" s="4">
-        <v>70</v>
-      </c>
-      <c r="C17" s="4">
-        <f t="shared" ref="C17:C24" si="2">C16+C15</f>
-        <v>6</v>
-      </c>
-      <c r="D17" s="4">
-        <f t="shared" ref="D17:D24" si="3">D16+10</f>
-        <v>88</v>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="5">
+        <v>37382.81</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1">
         <v>8000</v>
       </c>
-      <c r="B18" s="4">
-        <v>80</v>
-      </c>
-      <c r="C18" s="4">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="D18" s="4">
-        <f t="shared" si="3"/>
-        <v>98</v>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="5">
+        <v>232937.5</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1">
         <v>16000</v>
       </c>
-      <c r="B19" s="4">
-        <v>90</v>
-      </c>
-      <c r="C19" s="4">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="D19" s="4">
-        <f t="shared" si="3"/>
-        <v>108</v>
-      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1">
         <v>32000</v>
       </c>
-      <c r="B20" s="4">
-        <v>100</v>
-      </c>
-      <c r="C20" s="4">
-        <f t="shared" si="2"/>
-        <v>26</v>
-      </c>
-      <c r="D20" s="4">
-        <f t="shared" si="3"/>
-        <v>118</v>
-      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1">
         <v>64000</v>
       </c>
-      <c r="B21" s="4">
-        <v>110</v>
-      </c>
-      <c r="C21" s="4">
-        <f t="shared" si="2"/>
-        <v>42</v>
-      </c>
-      <c r="D21" s="4">
-        <f t="shared" si="3"/>
-        <v>128</v>
-      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1">
         <v>128000</v>
       </c>
-      <c r="B22" s="4">
-        <v>120</v>
-      </c>
-      <c r="C22" s="4">
-        <f t="shared" si="2"/>
-        <v>68</v>
-      </c>
-      <c r="D22" s="4">
-        <f t="shared" si="3"/>
-        <v>138</v>
-      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1">
         <v>256000</v>
       </c>
-      <c r="B23" s="4">
-        <v>130</v>
-      </c>
-      <c r="C23" s="4">
-        <f t="shared" si="2"/>
-        <v>110</v>
-      </c>
-      <c r="D23" s="4">
-        <f t="shared" si="3"/>
-        <v>148</v>
-      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1">
         <v>512000</v>
       </c>
-      <c r="B24" s="4">
-        <v>140</v>
-      </c>
-      <c r="C24" s="4">
-        <f t="shared" si="2"/>
-        <v>178</v>
-      </c>
-      <c r="D24" s="4">
-        <f t="shared" si="3"/>
-        <v>158</v>
-      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8191,9 +7886,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8408,19 +8106,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8445,9 +8139,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>